<commit_message>
Added styling changes + copy and images for demo dialog + tweaks for deployment
</commit_message>
<xml_diff>
--- a/Api/Augustus.Api/DemoTransactions.xlsx
+++ b/Api/Augustus.Api/DemoTransactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Augustus\Api\Augustus.Api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F85A13-83E6-4344-BCA6-C37522B100A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B650F27B-5184-4D23-AB2F-17F2FDF61D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E6207720-2DDE-493D-8786-838BB8C144C4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="52">
   <si>
     <t>Transaction date</t>
   </si>
@@ -172,6 +172,27 @@
   </si>
   <si>
     <t>Archery Club Membership</t>
+  </si>
+  <si>
+    <t>Hotel in Madrid</t>
+  </si>
+  <si>
+    <t>Cineworld</t>
+  </si>
+  <si>
+    <t>Cinema</t>
+  </si>
+  <si>
+    <t>M+L Electricity</t>
+  </si>
+  <si>
+    <t>Cooker repair</t>
+  </si>
+  <si>
+    <t>Light bulb</t>
+  </si>
+  <si>
+    <t>Fan from Amazon</t>
   </si>
 </sst>
 </file>
@@ -527,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96C5346-6CE8-48FD-922F-768D0FB2935E}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +599,7 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>146.61000000000001</v>
+        <v>136.61000000000001</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -606,9 +627,6 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -669,9 +687,6 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -810,7 +825,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>247.67</v>
+        <v>227.67</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1025,7 +1040,7 @@
         <v>34</v>
       </c>
       <c r="D23">
-        <v>146.54</v>
+        <v>126.54</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1157,7 +1172,7 @@
         <v>40</v>
       </c>
       <c r="D29">
-        <v>128.65</v>
+        <v>54.99</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1485,6 +1500,702 @@
       </c>
       <c r="F44">
         <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45">
+        <v>35.99</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44683</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>216.35</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>44684</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>23.35</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>44685</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>158</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>44686</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>120</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>6</v>
+      </c>
+      <c r="G49">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>44689</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>32.32</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>44693</v>
+      </c>
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51">
+        <v>65.25</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>44697</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52">
+        <v>85</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>12</v>
+      </c>
+      <c r="G52">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>44700</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>23.36</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>44701</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>18.25</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55">
+        <v>24.99</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56">
+        <v>25.14</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57">
+        <v>35.36</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>44716</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>158</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>125</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>6</v>
+      </c>
+      <c r="G59">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>37.35</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>44724</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61">
+        <v>59.35</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B62" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D62">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>12</v>
+      </c>
+      <c r="G62">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>44731</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63">
+        <v>35.24</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>4</v>
+      </c>
+      <c r="G63">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>44732</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>25.36</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
+      </c>
+      <c r="G64">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>44735</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65">
+        <v>70</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>44736</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>38.35</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>44742</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67">
+        <v>45</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>44746</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>130</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>44750</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69">
+        <v>25.36</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>44754</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70">
+        <v>45.87</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>44758</v>
+      </c>
+      <c r="B71" t="s">
+        <v>48</v>
+      </c>
+      <c r="C71" t="s">
+        <v>50</v>
+      </c>
+      <c r="D71">
+        <v>15</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>12</v>
+      </c>
+      <c r="G71">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>44761</v>
+      </c>
+      <c r="B72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72">
+        <v>24.14</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>4</v>
+      </c>
+      <c r="G72">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>44762</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73">
+        <v>37.25</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>4</v>
+      </c>
+      <c r="G73">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>44765</v>
+      </c>
+      <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D74">
+        <v>12.99</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>44766</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75">
+        <v>24.32</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>44772</v>
+      </c>
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" t="s">
+        <v>51</v>
+      </c>
+      <c r="D76">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>44772</v>
+      </c>
+      <c r="B77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77">
+        <v>15</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>